<commit_message>
Changed soft deletes + refactor
</commit_message>
<xml_diff>
--- a/ExcelDBviaEntityFramework/Excel files/Signups.xlsx
+++ b/ExcelDBviaEntityFramework/Excel files/Signups.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Emiel.Nijhuis\source\repos\misc\ExcelDBviaEntityFramework\ExcelDBviaEntityFramework\Excel files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enijh\source\repos\ExcelDBviaEntityFramework\ExcelDBviaEntityFramework\Excel files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D5D04F0-DA3E-442E-AC20-E96772BA37D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DE845A2-782E-4A95-A5C4-BD5828DF9B95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Name</t>
   </si>
@@ -63,9 +63,6 @@
     <t>123-456-7890</t>
   </si>
   <si>
-    <t>Id</t>
-  </si>
-  <si>
     <t>er5t6y93</t>
   </si>
   <si>
@@ -73,6 +70,12 @@
   </si>
   <si>
     <t>9kce6j8w</t>
+  </si>
+  <si>
+    <t>Deleted_ý</t>
+  </si>
+  <si>
+    <t>Id_ý</t>
   </si>
 </sst>
 </file>
@@ -270,7 +273,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -549,73 +552,85 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.33203125" customWidth="1"/>
-    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="14.33203125" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B3" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C3" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="7">
         <v>1</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>2</v>
-      </c>
     </row>
-    <row r="2" spans="1:4" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="4" t="s">
+    <row r="4" spans="1:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="C4" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="D4" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="9">
+      <c r="E4" s="9">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Implemented signup ID (not EF id)
</commit_message>
<xml_diff>
--- a/ExcelDBviaEntityFramework/Excel files/Signups.xlsx
+++ b/ExcelDBviaEntityFramework/Excel files/Signups.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enijh\source\repos\ExcelDBviaEntityFramework\ExcelDBviaEntityFramework\Excel files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6880D6C5-0B04-4C73-903C-8C0D0057D72E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1C3D7DB-C64B-4A1C-B9FB-6A89DB80E3A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3120" yWindow="1932" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Name</t>
   </si>
@@ -79,6 +79,12 @@
   </si>
   <si>
     <t>555-5551</t>
+  </si>
+  <si>
+    <t>Id</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
@@ -134,9 +140,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -418,91 +426,104 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11" hidden="1" customWidth="1"/>
     <col min="2" max="2" width="12.44140625" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.5546875" customWidth="1"/>
-    <col min="5" max="5" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.44140625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5546875" customWidth="1"/>
+    <col min="6" max="6" width="13.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>9</v>
       </c>
       <c r="B2" t="b">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="3">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>13</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
       <c r="B3" t="b">
         <v>0</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
         <v>4</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>5</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>10</v>
       </c>
       <c r="B4" t="b">
         <v>0</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="3">
+        <v>3</v>
+      </c>
+      <c r="D4" t="s">
         <v>6</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>7</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>2</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:F1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>